<commit_message>
nmv 25 02 2024
</commit_message>
<xml_diff>
--- a/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.7.xlsx
+++ b/TS Jatai Ghanam Project/Stas table for TS 4.1 TO 4.7.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALL IMP DATA\GitHub\texts\TS Jatai Ghanam Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3FB6A9-E1DF-4574-BCE2-5CD247622D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD6535AE-F44C-4CA0-A669-1AE19D23DD7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2248,7 +2248,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2333,6 +2333,21 @@
       <color rgb="FF000000"/>
       <name val="BRH Malayalam"/>
       <family val="4"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2438,7 +2453,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="fill"/>
@@ -2539,6 +2554,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2822,8 +2842,8 @@
   <dimension ref="A1:M58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49:K58"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F51" sqref="F51:F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3746,11 +3766,11 @@
       <c r="C24" s="3">
         <v>0</v>
       </c>
-      <c r="D24" s="3">
-        <v>1</v>
-      </c>
-      <c r="E24" s="3">
-        <v>1</v>
+      <c r="D24" s="38">
+        <v>0</v>
+      </c>
+      <c r="E24" s="38">
+        <v>0</v>
       </c>
       <c r="F24" s="3">
         <v>3</v>
@@ -4684,13 +4704,13 @@
         <f t="shared" ref="C48:L48" si="0">SUM(C2:C47)</f>
         <v>52</v>
       </c>
-      <c r="D48" s="26">
+      <c r="D48" s="39">
         <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="E48" s="26">
+        <v>32</v>
+      </c>
+      <c r="E48" s="39">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F48" s="26">
         <f t="shared" si="0"/>
@@ -4757,8 +4777,8 @@
       <c r="E51" t="s">
         <v>14</v>
       </c>
-      <c r="F51">
-        <v>24</v>
+      <c r="F51" s="40">
+        <v>23</v>
       </c>
       <c r="J51">
         <f>F57</f>
@@ -4769,7 +4789,7 @@
       <c r="E52" t="s">
         <v>15</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="40">
         <v>9</v>
       </c>
       <c r="J52" s="1" t="s">
@@ -4788,7 +4808,7 @@
     <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F54">
         <f>SUM(F49:F53)</f>
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="J54" s="1" t="s">
         <v>17</v>
@@ -4800,7 +4820,7 @@
       </c>
       <c r="F55">
         <f>K48-F54</f>
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="J55">
         <f>J53-L48</f>
@@ -14807,47 +14827,47 @@
         <v>39</v>
       </c>
       <c r="B41" s="29">
-        <f>SUM(B2:B40)</f>
+        <f t="shared" ref="B41:L41" si="0">SUM(B2:B40)</f>
         <v>206</v>
       </c>
       <c r="C41" s="29">
-        <f>SUM(C2:C40)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="D41" s="29">
-        <f>SUM(D2:D40)</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="E41" s="29">
-        <f>SUM(E2:E40)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F41" s="29">
-        <f>SUM(F2:F40)</f>
+        <f t="shared" si="0"/>
         <v>114</v>
       </c>
       <c r="G41" s="29">
-        <f>SUM(G2:G40)</f>
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="H41" s="29">
-        <f>SUM(H2:H40)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I41" s="29">
-        <f>SUM(I2:I40)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="J41" s="29">
-        <f>SUM(J2:J40)</f>
+        <f t="shared" si="0"/>
         <v>1692</v>
       </c>
       <c r="K41" s="29">
-        <f>SUM(K2:K40)</f>
+        <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="L41" s="29">
-        <f>SUM(L2:L40)</f>
+        <f t="shared" si="0"/>
         <v>2210</v>
       </c>
     </row>
@@ -14958,8 +14978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:L8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15006,7 +15026,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="2:12" ht="102" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:12" ht="89.25" x14ac:dyDescent="0.2">
       <c r="B2" s="6" t="s">
         <v>18</v>
       </c>
@@ -15050,7 +15070,7 @@
         <v>26</v>
       </c>
       <c r="E3" s="13">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="F3" s="13">
         <v>1982</v>
@@ -15072,7 +15092,7 @@
       </c>
       <c r="L3" s="13">
         <f>SUM(E3:K3)</f>
-        <v>11188</v>
+        <v>11189</v>
       </c>
     </row>
     <row r="4" spans="2:12" ht="42.75" x14ac:dyDescent="0.2">
@@ -15111,7 +15131,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="5" spans="2:12" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" ht="71.25" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>29</v>
       </c>
@@ -15158,7 +15178,7 @@
         <v>31</v>
       </c>
       <c r="E6" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="13">
         <v>14</v>
@@ -15180,10 +15200,10 @@
       </c>
       <c r="L6" s="13">
         <f>SUM(E6:K6)</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="42.75" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="54" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>32</v>
       </c>
@@ -15226,35 +15246,35 @@
         <v>23</v>
       </c>
       <c r="E8" s="17">
-        <f>SUM(E3:E7)</f>
+        <f t="shared" ref="E8:K8" si="0">SUM(E3:E7)</f>
         <v>2293</v>
       </c>
       <c r="F8" s="17">
-        <f>SUM(F3:F7)</f>
+        <f t="shared" si="0"/>
         <v>2498</v>
       </c>
       <c r="G8" s="17">
-        <f>SUM(G3:G7)</f>
+        <f t="shared" si="0"/>
         <v>1844</v>
       </c>
       <c r="H8" s="17">
-        <f>SUM(H3:H7)</f>
+        <f t="shared" si="0"/>
         <v>1887</v>
       </c>
       <c r="I8" s="17">
-        <f>SUM(I3:I7)</f>
+        <f t="shared" si="0"/>
         <v>1234</v>
       </c>
       <c r="J8" s="17">
-        <f>SUM(J3:J7)</f>
+        <f t="shared" si="0"/>
         <v>2331</v>
       </c>
       <c r="K8" s="17">
-        <f>SUM(K3:K7)</f>
+        <f t="shared" si="0"/>
         <v>2008</v>
       </c>
       <c r="L8" s="17">
-        <f t="shared" ref="L8" si="0">SUM(L3:L7)</f>
+        <f t="shared" ref="L8" si="1">SUM(L3:L7)</f>
         <v>14095</v>
       </c>
     </row>
@@ -15338,7 +15358,7 @@
         <v>35</v>
       </c>
       <c r="E14" s="13">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="F14" s="13">
         <v>1982</v>
@@ -15360,10 +15380,10 @@
       </c>
       <c r="L14" s="13">
         <f>SUM(E14:K14)</f>
-        <v>11188</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" ht="42.75" x14ac:dyDescent="0.3">
+        <v>11189</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="57" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>27</v>
       </c>
@@ -15446,7 +15466,7 @@
         <v>36</v>
       </c>
       <c r="E17" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="13">
         <v>14</v>
@@ -15468,7 +15488,7 @@
       </c>
       <c r="L17" s="13">
         <f>SUM(E17:K17)</f>
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="2:12" ht="85.5" x14ac:dyDescent="0.2">
@@ -15518,31 +15538,31 @@
         <v>2293</v>
       </c>
       <c r="F19" s="17">
-        <f t="shared" ref="F19:L19" si="1">SUM(F14:F18)</f>
+        <f t="shared" ref="F19:L19" si="2">SUM(F14:F18)</f>
         <v>2498</v>
       </c>
       <c r="G19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1844</v>
       </c>
       <c r="H19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1887</v>
       </c>
       <c r="I19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1234</v>
       </c>
       <c r="J19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2331</v>
       </c>
       <c r="K19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2008</v>
       </c>
       <c r="L19" s="17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>14095</v>
       </c>
     </row>
@@ -15626,7 +15646,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="13">
-        <v>1824</v>
+        <v>1825</v>
       </c>
       <c r="F25" s="13">
         <v>1982</v>
@@ -15648,7 +15668,7 @@
       </c>
       <c r="L25" s="13">
         <f>SUM(E25:K25)</f>
-        <v>11188</v>
+        <v>11189</v>
       </c>
     </row>
     <row r="26" spans="2:12" ht="82.5" x14ac:dyDescent="0.4">
@@ -15687,7 +15707,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="27" spans="2:12" ht="115.5" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:12" ht="132" x14ac:dyDescent="0.4">
       <c r="B27" s="12" t="s">
         <v>29</v>
       </c>
@@ -15734,7 +15754,7 @@
         <v>40</v>
       </c>
       <c r="E28" s="13">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F28" s="13">
         <v>14</v>
@@ -15756,10 +15776,10 @@
       </c>
       <c r="L28" s="13">
         <f>SUM(E28:K28)</f>
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="2:12" ht="115.5" x14ac:dyDescent="0.4">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="132" x14ac:dyDescent="0.4">
       <c r="B29" s="12" t="s">
         <v>32</v>
       </c>
@@ -15806,31 +15826,31 @@
         <v>2293</v>
       </c>
       <c r="F30" s="17">
-        <f t="shared" ref="F30" si="2">SUM(F25:F29)</f>
+        <f t="shared" ref="F30" si="3">SUM(F25:F29)</f>
         <v>2498</v>
       </c>
       <c r="G30" s="17">
-        <f t="shared" ref="G30" si="3">SUM(G25:G29)</f>
+        <f t="shared" ref="G30" si="4">SUM(G25:G29)</f>
         <v>1844</v>
       </c>
       <c r="H30" s="17">
-        <f t="shared" ref="H30" si="4">SUM(H25:H29)</f>
+        <f t="shared" ref="H30" si="5">SUM(H25:H29)</f>
         <v>1887</v>
       </c>
       <c r="I30" s="17">
-        <f t="shared" ref="I30" si="5">SUM(I25:I29)</f>
+        <f t="shared" ref="I30" si="6">SUM(I25:I29)</f>
         <v>1234</v>
       </c>
       <c r="J30" s="17">
-        <f t="shared" ref="J30" si="6">SUM(J25:J29)</f>
+        <f t="shared" ref="J30" si="7">SUM(J25:J29)</f>
         <v>2331</v>
       </c>
       <c r="K30" s="17">
-        <f t="shared" ref="K30" si="7">SUM(K25:K29)</f>
+        <f t="shared" ref="K30" si="8">SUM(K25:K29)</f>
         <v>2008</v>
       </c>
       <c r="L30" s="17">
-        <f t="shared" ref="L30" si="8">SUM(L25:L29)</f>
+        <f t="shared" ref="L30" si="9">SUM(L25:L29)</f>
         <v>14095</v>
       </c>
     </row>

</xml_diff>